<commit_message>
update script e artigos
</commit_message>
<xml_diff>
--- a/04_teoria/fichamentos_revisaoempirica.xlsx
+++ b/04_teoria/fichamentos_revisaoempirica.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP I3\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e94e91ad3b9f2a1e/Documentos/LAPEI-CIGETS/GitHub/tcp/04_teoria/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_033BD62EAC37CBAFCAA82BD66F7A2C0C8B5C2EA3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87C32D09-5A1E-4305-A325-46E7A024CFCA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -22,21 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Autores</t>
   </si>
@@ -63,9 +55,6 @@
   </si>
   <si>
     <t>Em termos de satisfação no trabalho, os padrões de trabalho autônomo persistentes tiveram a maior satisfação média no trabalho de 7,41, enquanto os de necessidade tiveram a menor satisfação média no trabalho de 6,78. Os padrões de trabalho autônomo persistentes também tiveram a maior satisfação média com a vida de 7,19 e os padrões de trabalho autônomo por necessidade tiveram a menor satisfação média com a vida de 6,82.</t>
-  </si>
-  <si>
-    <t>É utilizado dados do Painel Socioeconômico Alemão (SOEP) do período que compreende os anos de 1991 a 2016 de indivíduos que tiveram experiência com trabalho autônomo, excluído os agricultores e ajudantes em empresa familiar, totalizando uma amostra de 205 pessoas. Para identificação dos padrões foi empregado o método da análise de sequência com a técnica OMspell para medição de dissimilaridades e ligação de Ward para clusterização. Os autores reconheceram quatro clusters de carreira de trabalho por conta própria denominados: padrões mistos (33% da amostra), padrões por necessidade (29% da amostra), padrões intermitentes (24% da amostra) e padrões persistente (14% da amostra). Os autores testaram a hipótese através da análise de regressão de mínimos quadrados generalizados, utilizando como variáveis proxy de sucesso: a renda bruta, satisfação com o trabalho e satistação com a vida.</t>
   </si>
   <si>
     <t>Principais resultados descritivos</t>
@@ -222,9 +211,6 @@
     <t>https://doi.org/10.1007/s00168-022-01139-5</t>
   </si>
   <si>
-    <t>Análise de sequência e Regressão Multonomia</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1007/s10645-020-09358-x</t>
   </si>
   <si>
@@ -246,12 +232,6 @@
     <t>Analisar como as preocupações empreendedoras ao se tornar autônomo impacta na satisfação geral com a vida.</t>
   </si>
   <si>
-    <t>É utilizado dados do Painel Socioeconômico Alemão (SOEP) compreendendo o período 1984-2020. Foram selecionados indivíduos que desenvolveram trabalho autônomo em tempo integral com idade entre 17 e 65 anos e excluída as atividades de ajudante em empresa familiar e agricultor, resultando em uma amostra de 2.015 pessoas. Para testar as hipóteses é instrumentalizado um modelo de Regressões Aparentemente Não Relacionadas (SUR). A variável dependente é a satisfação com a vida e a variável independente de interesse é a que marca a transição para o trabalho autônomo. O método ainda tem como componente relevante uma variável mediadora, preocupações empreendedoras, por meio do qual se busca estimar um efeito de se tornar autônomo sobre a preocupação empreendedora e o seu consequente impacto sobre a satisfação com a vida. Para neutralizar o efeito da idade sobre a satisfação, é incluído um grupo de controle que não são autônomos, mas que se assemelham à esses. As variáveis de controle são: escolaridade, idade, estado civil, tipo de domicílio, deficiência, nacionalidade e personalidade.</t>
-  </si>
-  <si>
-    <t>A preocupação empreendedora é decomposta em três variáveis: preocupações com o desenvolvimento econômico, situação financeira e segurança do emprego. Além dessas variáveis, a renda e horas trabalhadas também foram agregadas como mediadoras no modelo. Os resultados mostraram que migrar para o trabalho autônomo têm um efeito indireto negativo na satisfação com a vida através das variáveis preocupações financeira (b = -0,05) e horas de trabalho (b = -0,04), e positivamente com a segurança no emprego (b = 0,01). A renda só foi significativa em um modelo alternativo construído com um grupo de controle menos restrito com um coeficiente de 0,01, mas ainda menor que preocupações financeiras que teve o mesmo efeito anterior. Indicando que a percepção subjetiva com as finanças tem um influência maior que a mudança objetiva de renda. Os efeitos opostos de se tornar autônomo sobre as preocupações com a segurança no emprego e a situação financeira, positivamente e negativamente, respectivamente, podem explicar um efeito geral da migração para autônomo estatísticamente não significativo sobre a satisfação com a vida (efeito direto).</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1016/j.joep.2024.102773</t>
   </si>
   <si>
@@ -259,12 +239,63 @@
   </si>
   <si>
     <t>O estudo fornece evidência de um efeito mediador das variáveis subjetivas (preocupações empreendedoras) sobre a satisfação com a vida, e confirma a heterogenidade ao se deparar com resultados distintos ao desagregar por tipos de autônomos. No entanto, dada as limitações da pesquisa, os resultados devem ser lidos como evidências e não uma relação de causalidade.</t>
+  </si>
+  <si>
+    <t>Em uma análise adicional, no qual é feita a interação da variáveis de trabalho autônomo com diferentes níveis de preocupações, mostrou o trabalho autônomo está positivamente relacionado com a satisfação de vida na ausência das preocupações empreendedoras. E ao inserir essas variáveis em níveis maiores, anulam o efeito sobre a satisfação.</t>
+  </si>
+  <si>
+    <t>Regressões Aparentemente Não Relacionadas (SUR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Os resultados mostraram que migrar para o trabalho autônomo têm um efeito indireto negativo na satisfação com a vida através das variáveis preocupações financeira (b = -0,05) e horas de trabalho (b = -0,04), e positivamente com a segurança no emprego (b = 0,01). A renda só foi significativa em um modelo alternativo construído com um grupo de controle menos restrito com um coeficiente de 0,01, mas ainda menor que preocupações financeiras que teve o mesmo efeito anterior. Indicando que a percepção subjetiva com as finanças tem um influência maior que a mudança objetiva de renda. Os efeitos opostos de se tornar autônomo sobre as preocupações com a segurança no emprego e a situação financeira, positivamente e negativamente, respectivamente, podem explicar um efeito geral da migração para autônomo estatísticamente não significativo sobre a satisfação com a vida (efeito direto).</t>
+  </si>
+  <si>
+    <t>É utilizado dados do Painel Socioeconômico Alemão (SOEP) compreendendo o período 1984-2020. Foram selecionados indivíduos que desenvolveram trabalho autônomo em tempo integral com idade entre 17 e 65 anos e excluída as atividades de ajudante em empresa familiar e agricultor, resultando em uma amostra de 2.015 pessoas. Para testar as hipóteses é instrumentalizado um modelo de Regressões Aparentemente Não Relacionadas (SUR). A variável dependente é a satisfação com a vida e a variável independente de interesse é a que marca a transição para o trabalho autônomo. O método ainda tem como componente mediador as preocupações empreendedoras, por meio do qual se busca estimar um efeito de se tornar autônomo sobre a preocupação empreendedora e o seu consequente impacto sobre a satisfação com a vida.A preocupação empreendedora é decomposta em três variáveis: preocupações com o desenvolvimento econômico, situação financeira e segurança do emprego. Além dessas variáveis, a renda e horas trabalhadas também foram agregadas como mediadoras no modelo. Para neutralizar o efeito da idade sobre a satisfação, é incluído um grupo de controle que não são autônomos, mas que se assemelham à esses. As variáveis de controle são: escolaridade, idade, estado civil, tipo de domicílio, deficiência, nacionalidade e personalidade.</t>
+  </si>
+  <si>
+    <t>O estudo tem como objetivo analisar o impacto de se tornar autônomo sobre a satisfação com a vida e verificar se as preocupações empreendedoras exercem papel mediador. A heterogeneidade também é analisada a luz das motivações, definindo os autônomos por oportunidade e necessidade. É utilizado dados do Painel Socioeconômico Alemão (SOEP) compreendendo o período 1984-2020. Foram selecionados indivíduos que desenvolveram trabalho autônomo em tempo integral com idade entre 17 e 65 anos e excluída as atividades de ajudante em empresa familiar e agricultor, resultando em uma amostra de 2.015 pessoas. Para testar as hipóteses é instrumentalizado um modelo de Regressões Aparentemente Não Relacionadas (SUR). A variável dependente é a satisfação com a vida e a variável independente de interesse é a que marca a transição para o trabalho autônomo. O método ainda tem como componente mediador, por meio do qual se busca estimar um efeito de se tornar autônomo sobre a preocupação empreendedora e o seu consequente impacto sobre a satisfação com a vida. A preocupação empreendedora é decomposta em três variáveis: preocupações com o desenvolvimento econômico, situação financeira e segurança do emprego. Além dessas variáveis, a renda e horas trabalhadas também foram agregadas como mediadoras no modelo. Os resultados mostraram que migrar para o trabalho autônomo têm um efeito indireto negativo na satisfação com a vida através das variáveis preocupações financeira (b = -0,05) e horas de trabalho (b = -0,04), e positivamente com a segurança no emprego (b = 0,01). Os efeitos opostos de se tornar autônomo sobre as preocupações com a segurança no emprego e a situação financeira, positivamente e negativamente, respectivamente, podem explicar um efeito geral da migração para autônomo estatisticamente não significativo sobre a satisfação com a vida (efeito direto). Na análise de heterogenidade desagregada por motivações de se tornar autônomo, foi observado, que no caso dos autônomos por oportunidade, há um efeito indireto positivo na satisfação com a vida através da variáveis segurança no emprego (b = 0,01) e na renda (b = 0,02), e horas de trabalho (b = -0,04), mas um efeito direto de se tornar autônomo não significativo. Por outro lado, os autônomos por necessidade, experimentaram um efeito direto significativo sobre a satisfação com a vida (b = 0,71), e indireto com preocupações financeiras (b = 0,19). O estudo fornece evidência de um efeito mediador das variáveis subjetivas (preocupações empreendedoras) sobre a satisfação com a vida, e confirma a heterogenidade ao se deparar com resultados distintos ao desagregar por tipos de autônomos. No entanto, dada as limitações da pesquisa, os resultados devem ser lidos como evidências e não uma relação de causalidade.</t>
+  </si>
+  <si>
+    <t>Sun, Jin e Zhao (2023)</t>
+  </si>
+  <si>
+    <t>Identificar tipologias de empreendedores chiseses e seus respectivos efeitos de saúde e econômicos.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1332/175795921X16889785709088</t>
+  </si>
+  <si>
+    <t>É utilizado dados do Estudo Longitudinal da Saúde e Aposentadoria na China (CHARLS) de indivíduos com mais de 45 anos coletados no ano de 2014 com uma perspectiva retrospectiva do histórico de vida, uma amostral total de 18.723 pessoas. Foram selecionados aqueles que exerceram trabalho autônomo não agrícola como a última atividade profissional. A classificação de autônomos adotada abrange com e sem empregados. Para identificar os padrões de carreira rumo ao empreendedorismo, foi empregado o método de análise de cluster com a técnica optimal matching para medição de dissimilaridades. As hipóteses são estadas através de modelos de mínimos quadrados ordinários construídos com três variáveis dependentes: autoavaliação de saúde (de 1 a 5), depressão (escore de questionário variando de 0 a 30) e renda (valor líquido). As variáveis de controle foram: gênero, idade, idade ao quadrado, estado civil, porcentagem de trabalho autônomo, anos de escolaridade, coorte de entrada no empreendedorismo, preditores da infância, local de residência e status atual do hukou.O número de clusters foram definidos apoiados pelas métricas pseudo-F de Calinski e Harabasz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foram definidos quatro clusters com as respectivas proporções em parênteses: (1) empreendedores agricultores (45,48%), (2) empreendedores persistentes (20,40%), (3) empreendedores por necessidade (17,25%) e (4) empreendedores empregados (16,87%). No entanto, dada a heterogenidade do cluster por necessidade, o autor prossegue a análise apenas com os demais grupos por serem mais comparáveis. Mas no que tange aos dados descritivos, é observado que mulheres é maioria (57,51%), enquanto nos clusters 1, 2 e 4 a proporção é de 37,02%. Com relação a idade, a média entre os autônomos por necessidade é de 50,4 anos e de empreendedores persistentes (48,20), empreendedores empregados (53,11) e empreendedores agricultores (55,23). Os autônomos por necessidade tem percentual superior aos demais em áreas urbanas hukou não agrícola. Com relação ao percentual de casados e os anos de escolaridade são similares. </t>
+  </si>
+  <si>
+    <t>A diferença de idade pode ser atribuída ao modelo de mobilidade social, cujo a frequência de empreendedores são maiores em estratos sociais mais elevados.</t>
+  </si>
+  <si>
+    <t>Análise de sequência e Regressão Multonomial</t>
+  </si>
+  <si>
+    <t>Em termos econômicos, representado pela renda, não houve diferença significativa entre os três clusters, assim como o percentual de tempo dedicado ao trabalho autônomo (no entanto, o output na tabela mostra essa variável significativa). Enquanto a renda e o estado civil de casado são positivamente associados à renda e o  hukou (registro de domicílio) não agrícola na infância está negativamente associado à renda.</t>
+  </si>
+  <si>
+    <t>Os resultados com relação à saúde, mostrou que os agricultores apresentaram a pior autoavaliação de saúde e os autônomos empregados e persistentes não diferiram. O resultado é atribuído a tipicidade do trabalho agrícola, por ser mais pesado, apresenta impactos prejudiciais de saúde no longo prazo. O percentual de tempo de trabalho autônomo não apresentou efeito significativo na saúde autoavaliada. Os homens têm resultado de saúde significativamente maiores que as mulheres. Com relação ao segundo indicador de saúde, a depressão, não foi encontrada diferença entre os três clusters. De acordo com o estudo, os resultados convergem, respectivamente, com as teorias vantagens acumulativas e do ponto de ajuste para análise autoavaliação de saúde, e escore de depressão e renda.</t>
+  </si>
+  <si>
+    <t>Em síntese, as evidências mostram relação das tipologias com a saúde dos autônomos, sendo os com experiência pregressa na agricultura com o pior resultado. No entanto, em termos econômicos, não foi encontrado diferença significativa entre as trajetórias de carreiras.</t>
+  </si>
+  <si>
+    <t>Análise de Sequência e Mínimos Quadrados Ordinários</t>
+  </si>
+  <si>
+    <t>É utilizado dados do Painel Socioeconômico Alemão (SOEP) do período que compreende os anos de 1991 a 2016 de indivíduos alemães que tiveram experiência com trabalho autônomo, excluído os agricultores e ajudantes em empresa familiar, totalizando uma amostra de 205 pessoas. Para identificação dos padrões foi empregado o método da análise de sequência com a técnica OMspell para medição de dissimilaridades e ligação de Ward para clusterização. Os autores reconheceram quatro clusters de carreira de trabalho por conta própria denominados: padrões mistos (33% da amostra), padrões por necessidade (29% da amostra), padrões intermitentes (24% da amostra) e padrões persistente (14% da amostra). Os autores testaram a hipótese através da análise de regressão de mínimos quadrados generalizados, utilizando como variáveis proxy de sucesso: a renda bruta, satisfação com o trabalho e satistação com a vida.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -338,7 +369,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -355,7 +386,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -364,7 +395,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -383,12 +414,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -704,17 +729,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="1" width="18" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="46" style="3" customWidth="1"/>
     <col min="4" max="4" width="88.28515625" style="3" customWidth="1"/>
@@ -727,7 +752,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -739,24 +764,24 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>66</v>
+      <c r="A2" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>5</v>
@@ -765,26 +790,26 @@
         <v>6</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>29</v>
+        <v>14</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="12"/>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -792,284 +817,371 @@
         <v>8</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+        <v>15</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="4" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="12"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
       <c r="E4" s="13"/>
       <c r="F4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
+        <v>16</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="12"/>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
       <c r="G5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="16" t="s">
+      <c r="C6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="F6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" ht="177.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-    </row>
-    <row r="9" spans="1:9" ht="177.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="10" t="s">
+      <c r="C9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="H9" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="10" t="s">
+      <c r="G12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" ht="300" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-    </row>
-    <row r="12" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-    </row>
-    <row r="13" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-    </row>
-    <row r="14" spans="1:9" ht="300" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-    </row>
-    <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-    </row>
-    <row r="16" spans="1:9" ht="195" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="C16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="I16" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="10" t="s">
+    </row>
+    <row r="17" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="I17" s="9"/>
     </row>
-    <row r="18" spans="1:9" ht="390" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+    <row r="18" spans="1:9" ht="300" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I18" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="7" t="s">
+    </row>
+    <row r="19" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I18" s="18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="210" x14ac:dyDescent="0.25">
-      <c r="F19" s="4" t="s">
-        <v>72</v>
-      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" ht="261" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="43">
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="I9:I15"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="A16:A17"/>
-    <mergeCell ref="C9:C15"/>
-    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="D9:D15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="H9:H15"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="H6:H8"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A15"/>
@@ -1082,26 +1194,25 @@
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="G6:G8"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="I9:I15"/>
-    <mergeCell ref="I6:I8"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="D9:D15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="H9:H15"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="C9:C15"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B21:B22"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I16" r:id="rId1"/>
-    <hyperlink ref="I9" r:id="rId2"/>
-    <hyperlink ref="I6" r:id="rId3"/>
-    <hyperlink ref="I2" r:id="rId4"/>
-    <hyperlink ref="I18" r:id="rId5"/>
+    <hyperlink ref="I16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="I6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="I2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="I18" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="I21" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>